<commit_message>
Commiting work as of 12/02/20 11:55 PM.
</commit_message>
<xml_diff>
--- a/Urbest/Testdata/TestDataUrbest.xlsx
+++ b/Urbest/Testdata/TestDataUrbest.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="24">
   <si>
     <t xml:space="preserve">URL</t>
   </si>
@@ -63,10 +63,37 @@
     <t xml:space="preserve">Firefox</t>
   </si>
   <si>
+    <t xml:space="preserve">Remote</t>
+  </si>
+  <si>
     <t xml:space="preserve">Opera</t>
   </si>
   <si>
     <t xml:space="preserve">Title</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Popup messages</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Username</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Login – UR BEST COACH PTY LTD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wrong username or password.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Login successful,redirecting…</t>
+  </si>
+  <si>
+    <t xml:space="preserve">uSER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">abc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fkdsjfksf</t>
   </si>
 </sst>
 </file>
@@ -76,11 +103,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -117,6 +145,20 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="9"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -167,7 +209,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -186,6 +228,26 @@
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -268,7 +330,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="89" zoomScaleNormal="89" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
+      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -324,12 +386,14 @@
       <c r="D3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="2"/>
+      <c r="E3" s="2" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4"/>
       <c r="D4" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -354,23 +418,24 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="89" zoomScaleNormal="89" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.63"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -383,20 +448,93 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="89" zoomScaleNormal="89" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.06"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="11.52"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="21.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="8"/>
+      <c r="B3" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="8"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="8"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="8" t="n">
+        <v>123456</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="8"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>